<commit_message>
excel demo file for student bulk import
</commit_message>
<xml_diff>
--- a/public/assets/files/Student_Demo_File.xlsx
+++ b/public/assets/files/Student_Demo_File.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\wamp64\www\jisha\AIMS\public\assets\files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\TOMSHER\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC190EC7-025E-4199-B884-BE51C17CC1D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EBC12B33-7988-433B-82AA-38355B80FB30}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{5BAB79A4-8846-4623-8977-6A882686E734}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>First Name</t>
   </si>
@@ -56,6 +56,22 @@
   <si>
     <t>DOB (YYYY-MM-DD)</t>
   </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Student Code </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(Optional)</t>
+    </r>
+  </si>
 </sst>
 </file>
 
@@ -64,7 +80,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd;@"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -90,6 +106,14 @@
     </font>
     <font>
       <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -449,10 +473,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B61D152C-2F6E-4A60-8EBC-F448EB779BC3}">
-  <dimension ref="A1:H34"/>
+  <dimension ref="A1:H26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="F1" sqref="F1:F1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -464,6 +488,7 @@
     <col min="5" max="5" width="23.5703125" customWidth="1"/>
     <col min="6" max="6" width="23.5703125" style="6" customWidth="1"/>
     <col min="7" max="7" width="35.7109375" customWidth="1"/>
+    <col min="8" max="8" width="27" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
@@ -488,7 +513,9 @@
       <c r="G1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="H1" s="2"/>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="2"/>
@@ -503,7 +530,7 @@
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="2"/>
       <c r="B3" s="2"/>
-      <c r="C3" s="3"/>
+      <c r="C3" s="2"/>
       <c r="D3" s="2"/>
       <c r="E3" s="2"/>
       <c r="F3" s="4"/>
@@ -513,7 +540,7 @@
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="2"/>
       <c r="B4" s="2"/>
-      <c r="C4" s="3"/>
+      <c r="C4" s="2"/>
       <c r="D4" s="2"/>
       <c r="E4" s="2"/>
       <c r="F4" s="4"/>
@@ -523,7 +550,7 @@
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="2"/>
       <c r="B5" s="2"/>
-      <c r="C5" s="3"/>
+      <c r="C5" s="2"/>
       <c r="D5" s="2"/>
       <c r="E5" s="2"/>
       <c r="F5" s="4"/>
@@ -533,7 +560,7 @@
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="2"/>
       <c r="B6" s="2"/>
-      <c r="C6" s="3"/>
+      <c r="C6" s="2"/>
       <c r="D6" s="2"/>
       <c r="E6" s="2"/>
       <c r="F6" s="4"/>
@@ -543,7 +570,7 @@
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="2"/>
       <c r="B7" s="2"/>
-      <c r="C7" s="3"/>
+      <c r="C7" s="2"/>
       <c r="D7" s="2"/>
       <c r="E7" s="2"/>
       <c r="F7" s="4"/>
@@ -553,7 +580,7 @@
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="2"/>
       <c r="B8" s="2"/>
-      <c r="C8" s="3"/>
+      <c r="C8" s="2"/>
       <c r="D8" s="2"/>
       <c r="E8" s="2"/>
       <c r="F8" s="4"/>
@@ -740,86 +767,6 @@
       <c r="G26" s="2"/>
       <c r="H26" s="2"/>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A27" s="2"/>
-      <c r="B27" s="2"/>
-      <c r="C27" s="2"/>
-      <c r="D27" s="2"/>
-      <c r="E27" s="2"/>
-      <c r="F27" s="4"/>
-      <c r="G27" s="2"/>
-      <c r="H27" s="2"/>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A28" s="2"/>
-      <c r="B28" s="2"/>
-      <c r="C28" s="2"/>
-      <c r="D28" s="2"/>
-      <c r="E28" s="2"/>
-      <c r="F28" s="4"/>
-      <c r="G28" s="2"/>
-      <c r="H28" s="2"/>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A29" s="2"/>
-      <c r="B29" s="2"/>
-      <c r="C29" s="2"/>
-      <c r="D29" s="2"/>
-      <c r="E29" s="2"/>
-      <c r="F29" s="4"/>
-      <c r="G29" s="2"/>
-      <c r="H29" s="2"/>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A30" s="2"/>
-      <c r="B30" s="2"/>
-      <c r="C30" s="2"/>
-      <c r="D30" s="2"/>
-      <c r="E30" s="2"/>
-      <c r="F30" s="4"/>
-      <c r="G30" s="2"/>
-      <c r="H30" s="2"/>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A31" s="2"/>
-      <c r="B31" s="2"/>
-      <c r="C31" s="2"/>
-      <c r="D31" s="2"/>
-      <c r="E31" s="2"/>
-      <c r="F31" s="4"/>
-      <c r="G31" s="2"/>
-      <c r="H31" s="2"/>
-    </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A32" s="2"/>
-      <c r="B32" s="2"/>
-      <c r="C32" s="2"/>
-      <c r="D32" s="2"/>
-      <c r="E32" s="2"/>
-      <c r="F32" s="4"/>
-      <c r="G32" s="2"/>
-      <c r="H32" s="2"/>
-    </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A33" s="2"/>
-      <c r="B33" s="2"/>
-      <c r="C33" s="2"/>
-      <c r="D33" s="2"/>
-      <c r="E33" s="2"/>
-      <c r="F33" s="4"/>
-      <c r="G33" s="2"/>
-      <c r="H33" s="2"/>
-    </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A34" s="2"/>
-      <c r="B34" s="2"/>
-      <c r="C34" s="2"/>
-      <c r="D34" s="2"/>
-      <c r="E34" s="2"/>
-      <c r="F34" s="4"/>
-      <c r="G34" s="2"/>
-      <c r="H34" s="2"/>
-    </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>